<commit_message>
Final Bugfixes - Working
</commit_message>
<xml_diff>
--- a/Excel/blankpythontester.xlsx
+++ b/Excel/blankpythontester.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:F110"/>
+  <dimension ref="A2:F118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1600,7 +1600,88 @@
       <c r="B110" t="n">
         <v>8.974591905842381</v>
       </c>
-      <c r="C110" t="inlineStr"/>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>0</v>
+      </c>
+      <c r="B111" t="n">
+        <v>8.308481844973947</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>0</v>
+      </c>
+      <c r="B112" t="n">
+        <v>8.308481844973947</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>0</v>
+      </c>
+      <c r="B113" t="n">
+        <v>8.308481844973947</v>
+      </c>
+      <c r="C113" t="n">
+        <v>0.08425404025794732</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>0</v>
+      </c>
+      <c r="B114" t="n">
+        <v>8.974591905842381</v>
+      </c>
+      <c r="C114" t="n">
+        <v>0.4632327957854892</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>0</v>
+      </c>
+      <c r="B115" t="n">
+        <v>8.974591905842381</v>
+      </c>
+      <c r="C115" t="n">
+        <v>0.4646062144118369</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>0</v>
+      </c>
+      <c r="B116" t="n">
+        <v>8.107829945440615</v>
+      </c>
+      <c r="C116" t="n">
+        <v>0.1754485456778251</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>0</v>
+      </c>
+      <c r="B117" t="n">
+        <v>8.039306644322307</v>
+      </c>
+      <c r="C117" t="n">
+        <v>0.8160774729312702</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>0</v>
+      </c>
+      <c r="B118" t="n">
+        <v>9.898999999999999</v>
+      </c>
+      <c r="C118" t="n">
+        <v>0.4042252753665664</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>